<commit_message>
Created Test File for Registration Module-Nishi
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -3,16 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{03949F87-5981-4E5D-A34D-4645F4A8E2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\DsalgoTestNg\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655F54B0-EA35-4F09-9302-A3674CC63616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>1@chicago</t>
   </si>
@@ -57,14 +63,59 @@
     <t>Y</t>
   </si>
   <si>
-    <t>qatitans78</t>
+    <t>TestUser01</t>
+  </si>
+  <si>
+    <t>Test@1234</t>
+  </si>
+  <si>
+    <t>Test@12346</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>invaliduser</t>
+  </si>
+  <si>
+    <t>77777777</t>
+  </si>
+  <si>
+    <t>7777777</t>
+  </si>
+  <si>
+    <t>TestUser04</t>
+  </si>
+  <si>
+    <t>www</t>
+  </si>
+  <si>
+    <t>Test@12349</t>
+  </si>
+  <si>
+    <t>@#$%#$#@</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>TestUser1</t>
+  </si>
+  <si>
+    <t>TestUser2</t>
+  </si>
+  <si>
+    <t>qatitans86</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,16 +137,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,12 +181,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -119,6 +227,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,7 +604,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -562,4 +682,158 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BF92DD-4B2C-45B6-9A36-15AB78A82F13}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D3829F-7C9E-4A7F-8E08-32F4F2BF4D32}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="4" width="14.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created Test files for Array module and updated Registration module
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\DsalgoTestNg\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655F54B0-EA35-4F09-9302-A3674CC63616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52893A2B-E0E6-4E4C-AA06-1A1E5E8CF8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="8170" firstSheet="2" activeTab="5" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>1@chicago</t>
   </si>
@@ -109,13 +111,46 @@
   </si>
   <si>
     <t>qatitans86</t>
+  </si>
+  <si>
+    <t>OptionOnArray</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Arrays in Python</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>NameError: name 'abcd' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Arrays using List</t>
+  </si>
+  <si>
+    <t>Basic Operations in Lists</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>print('Hello QATitans!')</t>
+  </si>
+  <si>
+    <t>Hello QATitans!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +192,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -216,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -239,6 +279,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -578,17 +627,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.5" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -602,7 +651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -634,14 +683,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -652,7 +701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -663,7 +712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -671,7 +720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -692,12 +741,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -708,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -719,7 +768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -730,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -741,7 +790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -752,7 +801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -776,14 +825,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.36328125" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" customWidth="1"/>
     <col min="3" max="4" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="28.5" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -797,7 +846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="28.5" thickBot="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>12</v>
@@ -809,7 +858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="28.5" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -821,7 +870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="28.5" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -836,4 +885,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA2490D-FDB4-4D02-9AB4-5ACD4FEED378}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D004443-7B75-4A96-95F4-63675E014615}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29">
+      <c r="A4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created test files for Stack and Login Modules - Madhura
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\DsalgoTestNg\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52893A2B-E0E6-4E4C-AA06-1A1E5E8CF8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BBCC44A7-9C22-4DBE-8200-B6A3913D7524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="8170" firstSheet="2" activeTab="5" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:U20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>1@chicago</t>
   </si>
@@ -111,46 +105,13 @@
   </si>
   <si>
     <t>qatitans86</t>
-  </si>
-  <si>
-    <t>OptionOnArray</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>Arrays in Python</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>NameError: name 'abcd' is not defined on line 1</t>
-  </si>
-  <si>
-    <t>Arrays using List</t>
-  </si>
-  <si>
-    <t>Basic Operations in Lists</t>
-  </si>
-  <si>
-    <t>Applications of Array</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>print('Hello QATitans!')</t>
-  </si>
-  <si>
-    <t>Hello QATitans!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,11 +153,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -256,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -279,15 +235,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -631,13 +578,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -651,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -679,18 +626,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -701,7 +648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -712,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -720,7 +667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -741,12 +688,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -757,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -768,7 +715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -779,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -790,7 +737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -801,7 +748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -825,14 +772,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="4" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" thickBot="1">
+    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -846,7 +793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" thickBot="1">
+    <row r="2" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>12</v>
@@ -858,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.5" thickBot="1">
+    <row r="3" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -870,7 +817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.5" thickBot="1">
+    <row r="4" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -885,155 +832,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA2490D-FDB4-4D02-9AB4-5ACD4FEED378}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="23.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="20.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D004443-7B75-4A96-95F4-63675E014615}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="29">
-      <c r="A4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Work in progress : changes to Login, Stack and Linked List Module
e
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -3,18 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BBCC44A7-9C22-4DBE-8200-B6A3913D7524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\eclipse-workspace\DSAlgo-TestNG\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD85DBB-E324-4AF8-9403-74524A578E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="1260" yWindow="2250" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="9" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
   <si>
     <t>1@chicago</t>
   </si>
@@ -105,6 +115,108 @@
   </si>
   <si>
     <t>qatitans86</t>
+  </si>
+  <si>
+    <t>OptionOnLinkedList</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Types of Linked List</t>
+  </si>
+  <si>
+    <t>Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>NameError: name 'abc123' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>print('Hello World! Creating Linked LIst')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Types of Linked List')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Implement Linked List in Python')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Traversal')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Insertion')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Deletion')</t>
+  </si>
+  <si>
+    <t>Hello World! Introduction</t>
+  </si>
+  <si>
+    <t>Hello World! Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Hello World! Types of Linked List</t>
+  </si>
+  <si>
+    <t>Hello World! Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Hello World! Traversal</t>
+  </si>
+  <si>
+    <t>Hello World! Insertion</t>
+  </si>
+  <si>
+    <t>Hello World! Deletion</t>
+  </si>
+  <si>
+    <t>print('Hello World! Introduction')</t>
+  </si>
+  <si>
+    <t>Operations in Stack</t>
+  </si>
+  <si>
+    <t>OptionOnStack</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Abcd</t>
+  </si>
+  <si>
+    <t>NameError: name 'Abcd' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>print('Hello World')</t>
+  </si>
+  <si>
+    <t>Hello World</t>
   </si>
 </sst>
 </file>
@@ -622,11 +734,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0C4824-5F65-4D5A-B959-3B0994E98AD4}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -832,4 +1008,306 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE770C-7909-4CE9-9774-C44C8979B4AA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7154BA82-7858-469B-9C9F-E2F02D223513}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A28EC0-BF7B-43E7-ADD7-3F79949FF775}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD6B667-CE06-461A-A71C-2657D9E05029}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161996F6-CCD1-43B0-93E3-022FC7F64E63}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Used PR#8 and added code for Home & DSIntro pages.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -3,18 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BBCC44A7-9C22-4DBE-8200-B6A3913D7524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\eclipse-workspace\DSAlgo-TestNG\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD85DBB-E324-4AF8-9403-74524A578E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="1260" yWindow="2250" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="9" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
   <si>
     <t>1@chicago</t>
   </si>
@@ -105,6 +115,108 @@
   </si>
   <si>
     <t>qatitans86</t>
+  </si>
+  <si>
+    <t>OptionOnLinkedList</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Types of Linked List</t>
+  </si>
+  <si>
+    <t>Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>NameError: name 'abc123' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>print('Hello World! Creating Linked LIst')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Types of Linked List')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Implement Linked List in Python')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Traversal')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Insertion')</t>
+  </si>
+  <si>
+    <t>print('Hello World! Deletion')</t>
+  </si>
+  <si>
+    <t>Hello World! Introduction</t>
+  </si>
+  <si>
+    <t>Hello World! Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Hello World! Types of Linked List</t>
+  </si>
+  <si>
+    <t>Hello World! Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Hello World! Traversal</t>
+  </si>
+  <si>
+    <t>Hello World! Insertion</t>
+  </si>
+  <si>
+    <t>Hello World! Deletion</t>
+  </si>
+  <si>
+    <t>print('Hello World! Introduction')</t>
+  </si>
+  <si>
+    <t>Operations in Stack</t>
+  </si>
+  <si>
+    <t>OptionOnStack</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Abcd</t>
+  </si>
+  <si>
+    <t>NameError: name 'Abcd' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>print('Hello World')</t>
+  </si>
+  <si>
+    <t>Hello World</t>
   </si>
 </sst>
 </file>
@@ -622,11 +734,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0C4824-5F65-4D5A-B959-3B0994E98AD4}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -832,4 +1008,306 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE770C-7909-4CE9-9774-C44C8979B4AA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7154BA82-7858-469B-9C9F-E2F02D223513}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A28EC0-BF7B-43E7-ADD7-3F79949FF775}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD6B667-CE06-461A-A71C-2657D9E05029}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161996F6-CCD1-43B0-93E3-022FC7F64E63}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated and changed files
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\eclipse-workspace\DSAlgo-TestNG\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD85DBB-E324-4AF8-9403-74524A578E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A8E3DFF0-7D00-4A49-B274-80683A54F7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2250" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="9" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="8" activeTab="10" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +18,11 @@
     <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="12" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="78">
   <si>
     <t>1@chicago</t>
   </si>
@@ -217,6 +215,57 @@
   </si>
   <si>
     <t>Hello World</t>
+  </si>
+  <si>
+    <t>OptionOnArray</t>
+  </si>
+  <si>
+    <t>Arrays in Python</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>NameError: name 'abcd' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Arrays using List</t>
+  </si>
+  <si>
+    <t>Basic Operations in Lists</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>print('Hello QATitans!')</t>
+  </si>
+  <si>
+    <t>Hello QATitans!</t>
+  </si>
+  <si>
+    <t>OptionOnTree</t>
+  </si>
+  <si>
+    <t>Overview of Trees</t>
+  </si>
+  <si>
+    <t>Terminologies</t>
+  </si>
+  <si>
+    <t>Types of Trees</t>
+  </si>
+  <si>
+    <t>Tree Traversals</t>
+  </si>
+  <si>
+    <t>Traversals-Illustration</t>
+  </si>
+  <si>
+    <t>Binary Trees</t>
+  </si>
+  <si>
+    <t>Types of Binary Trees</t>
   </si>
 </sst>
 </file>
@@ -690,13 +739,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -710,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -736,61 +785,304 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0C4824-5F65-4D5A-B959-3B0994E98AD4}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA07F58-65B4-4321-91B4-10A71ADF5AB6}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:Z1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8A3C36-F8FA-45CD-9A9A-4C09EFF2E799}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -806,14 +1098,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -824,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -835,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -843,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -864,12 +1156,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -880,7 +1172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -891,7 +1183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -902,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -913,7 +1205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -924,7 +1216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -948,14 +1240,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="4" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -969,7 +1261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>12</v>
@@ -981,7 +1273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -993,7 +1285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -1012,24 +1304,143 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE770C-7909-4CE9-9774-C44C8979B4AA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7154BA82-7858-469B-9C9F-E2F02D223513}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1042,13 +1453,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1070,7 +1481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1081,7 +1492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1092,7 +1503,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1103,7 +1514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1114,7 +1525,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1125,7 +1536,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1149,14 +1560,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1178,7 +1589,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1189,7 +1600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1200,7 +1611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1211,7 +1622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1222,7 +1633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1644,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1257,13 +1668,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1274,7 +1685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1285,7 +1696,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1296,7 +1707,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>55</v>
       </c>

</xml_diff>